<commit_message>
compiled week7 results and match files upto match #66
</commit_message>
<xml_diff>
--- a/final/overall_poll_margin.xlsx
+++ b/final/overall_poll_margin.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\meInspiron\Desktop\ipl_polls\final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2EFA45D-690F-4463-B4A2-8BD025ECB689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12826AF3-DDC4-4151-9FC8-6580F8B04E7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{153ECFA8-E1EE-4F9C-881D-7229152185BC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{153ECFA8-E1EE-4F9C-881D-7229152185BC}"/>
   </bookViews>
   <sheets>
-    <sheet name="Week6" sheetId="6" r:id="rId1"/>
+    <sheet name="Week8" sheetId="8" r:id="rId1"/>
+    <sheet name="Week7" sheetId="7" r:id="rId2"/>
+    <sheet name="Week6" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="130">
   <si>
     <t>Dense Rank</t>
   </si>
@@ -321,13 +323,118 @@
   </si>
   <si>
     <t>WEEZY F. Baby</t>
+  </si>
+  <si>
+    <t>Week7</t>
+  </si>
+  <si>
+    <t>Week8</t>
+  </si>
+  <si>
+    <t>—</t>
+  </si>
+  <si>
+    <t>↑1</t>
+  </si>
+  <si>
+    <t>↑5</t>
+  </si>
+  <si>
+    <t>↑3</t>
+  </si>
+  <si>
+    <t>↓1</t>
+  </si>
+  <si>
+    <t>↓2</t>
+  </si>
+  <si>
+    <t>↑17</t>
+  </si>
+  <si>
+    <t>↓4</t>
+  </si>
+  <si>
+    <t>Jason Duval</t>
+  </si>
+  <si>
+    <t>Beluga</t>
+  </si>
+  <si>
+    <t>↑7</t>
+  </si>
+  <si>
+    <t>↓7</t>
+  </si>
+  <si>
+    <t>oracle_priest</t>
+  </si>
+  <si>
+    <t>Sunny Paaji</t>
+  </si>
+  <si>
+    <t>_simplet0n</t>
+  </si>
+  <si>
+    <t>ZePHyR</t>
+  </si>
+  <si>
+    <t>↓5</t>
+  </si>
+  <si>
+    <t>ashmrth</t>
+  </si>
+  <si>
+    <t>Ashmrth</t>
+  </si>
+  <si>
+    <t>darkwolf_newbie</t>
+  </si>
+  <si>
+    <t>Darkwolf</t>
+  </si>
+  <si>
+    <t>dhanda_</t>
+  </si>
+  <si>
+    <t>Hank Schrader</t>
+  </si>
+  <si>
+    <t>elprofesor6338</t>
+  </si>
+  <si>
+    <t>Èl Profesor™</t>
+  </si>
+  <si>
+    <t>ind_mafia_sahil</t>
+  </si>
+  <si>
+    <t>IND_Mafia_Sahil</t>
+  </si>
+  <si>
+    <t>indianduder</t>
+  </si>
+  <si>
+    <t>boring-life</t>
+  </si>
+  <si>
+    <t>milkanananaannanan</t>
+  </si>
+  <si>
+    <t>Milk</t>
+  </si>
+  <si>
+    <t>vinnu7980</t>
+  </si>
+  <si>
+    <t>Vinnu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -346,6 +453,12 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
@@ -687,7 +800,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -749,6 +862,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -782,23 +909,115 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF002060"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEBF3FB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF002060"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEBF3FB"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1170,10 +1389,2371 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ACDE1E1-115B-4D8B-84AF-1822FA3E4DB8}">
+  <dimension ref="B1:K49"/>
+  <sheetViews>
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K46" sqref="B38:K46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="0.625" customWidth="1"/>
+    <col min="2" max="2" width="7.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="7.625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="21.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" style="2"/>
+    <col min="9" max="10" width="9" style="2" customWidth="1"/>
+    <col min="11" max="11" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" ht="4.5" customHeight="1" thickBot="1"/>
+    <row r="2" spans="2:11" ht="15.75" thickBot="1">
+      <c r="B2" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="33"/>
+    </row>
+    <row r="3" spans="2:11">
+      <c r="B3" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="35"/>
+      <c r="D3" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="37"/>
+      <c r="F3" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="J3" s="42" t="s">
+        <v>96</v>
+      </c>
+      <c r="K3" s="44" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="15.75" thickBot="1">
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="39"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="45"/>
+    </row>
+    <row r="5" spans="2:11" ht="14.25" customHeight="1">
+      <c r="B5" s="7"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="12"/>
+    </row>
+    <row r="6" spans="2:11" ht="14.25" customHeight="1">
+      <c r="B6" s="13"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="18"/>
+    </row>
+    <row r="7" spans="2:11" ht="15" customHeight="1">
+      <c r="B7" s="13"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="18"/>
+    </row>
+    <row r="8" spans="2:11">
+      <c r="B8" s="13"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="18"/>
+    </row>
+    <row r="9" spans="2:11">
+      <c r="B9" s="13"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="18"/>
+    </row>
+    <row r="10" spans="2:11">
+      <c r="B10" s="13"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="18"/>
+    </row>
+    <row r="11" spans="2:11">
+      <c r="B11" s="13"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="18"/>
+    </row>
+    <row r="12" spans="2:11">
+      <c r="B12" s="13"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="18"/>
+    </row>
+    <row r="13" spans="2:11">
+      <c r="B13" s="13"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="18"/>
+    </row>
+    <row r="14" spans="2:11">
+      <c r="B14" s="13"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="18"/>
+    </row>
+    <row r="15" spans="2:11" ht="14.25" customHeight="1">
+      <c r="B15" s="13"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="18"/>
+    </row>
+    <row r="16" spans="2:11" ht="14.25" customHeight="1">
+      <c r="B16" s="13"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="18"/>
+    </row>
+    <row r="17" spans="2:11" ht="14.25" customHeight="1">
+      <c r="B17" s="13"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="18"/>
+    </row>
+    <row r="18" spans="2:11" ht="14.25" customHeight="1">
+      <c r="B18" s="13"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="18"/>
+    </row>
+    <row r="19" spans="2:11">
+      <c r="B19" s="13"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="18"/>
+    </row>
+    <row r="20" spans="2:11">
+      <c r="B20" s="13"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="18"/>
+    </row>
+    <row r="21" spans="2:11">
+      <c r="B21" s="13"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="18"/>
+    </row>
+    <row r="22" spans="2:11">
+      <c r="B22" s="13"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="18"/>
+    </row>
+    <row r="23" spans="2:11">
+      <c r="B23" s="13"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="18"/>
+    </row>
+    <row r="24" spans="2:11">
+      <c r="B24" s="13"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17"/>
+      <c r="K24" s="18"/>
+    </row>
+    <row r="25" spans="2:11">
+      <c r="B25" s="13"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="17"/>
+      <c r="K25" s="18"/>
+    </row>
+    <row r="26" spans="2:11">
+      <c r="B26" s="13"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17"/>
+      <c r="K26" s="18"/>
+    </row>
+    <row r="27" spans="2:11">
+      <c r="B27" s="13"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="18"/>
+    </row>
+    <row r="28" spans="2:11">
+      <c r="B28" s="13"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="17"/>
+      <c r="K28" s="18"/>
+    </row>
+    <row r="29" spans="2:11">
+      <c r="B29" s="13"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="17"/>
+      <c r="J29" s="17"/>
+      <c r="K29" s="18"/>
+    </row>
+    <row r="30" spans="2:11">
+      <c r="B30" s="13"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="17"/>
+      <c r="J30" s="17"/>
+      <c r="K30" s="18"/>
+    </row>
+    <row r="31" spans="2:11">
+      <c r="B31" s="13"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="17"/>
+      <c r="J31" s="17"/>
+      <c r="K31" s="18"/>
+    </row>
+    <row r="32" spans="2:11">
+      <c r="B32" s="13"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="17"/>
+      <c r="I32" s="17"/>
+      <c r="J32" s="17"/>
+      <c r="K32" s="18"/>
+    </row>
+    <row r="33" spans="2:11">
+      <c r="B33" s="13"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="17"/>
+      <c r="J33" s="17"/>
+      <c r="K33" s="18"/>
+    </row>
+    <row r="34" spans="2:11">
+      <c r="B34" s="13"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="17"/>
+      <c r="J34" s="17"/>
+      <c r="K34" s="18"/>
+    </row>
+    <row r="35" spans="2:11">
+      <c r="B35" s="13"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="17"/>
+      <c r="J35" s="17"/>
+      <c r="K35" s="18"/>
+    </row>
+    <row r="36" spans="2:11">
+      <c r="B36" s="13"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="17"/>
+      <c r="I36" s="17"/>
+      <c r="J36" s="17"/>
+      <c r="K36" s="18"/>
+    </row>
+    <row r="37" spans="2:11">
+      <c r="B37" s="13"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="17"/>
+      <c r="I37" s="17"/>
+      <c r="J37" s="17"/>
+      <c r="K37" s="18"/>
+    </row>
+    <row r="38" spans="2:11">
+      <c r="B38" s="13"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="17"/>
+      <c r="I38" s="17"/>
+      <c r="J38" s="17"/>
+      <c r="K38" s="18"/>
+    </row>
+    <row r="39" spans="2:11">
+      <c r="B39" s="13"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="17"/>
+      <c r="I39" s="17"/>
+      <c r="J39" s="17"/>
+      <c r="K39" s="18"/>
+    </row>
+    <row r="40" spans="2:11">
+      <c r="B40" s="13"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="16"/>
+      <c r="H40" s="17"/>
+      <c r="I40" s="17"/>
+      <c r="J40" s="17"/>
+      <c r="K40" s="18"/>
+    </row>
+    <row r="41" spans="2:11">
+      <c r="B41" s="13"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="17"/>
+      <c r="I41" s="17"/>
+      <c r="J41" s="17"/>
+      <c r="K41" s="18"/>
+    </row>
+    <row r="42" spans="2:11">
+      <c r="B42" s="13"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="17"/>
+      <c r="I42" s="17"/>
+      <c r="J42" s="17"/>
+      <c r="K42" s="18"/>
+    </row>
+    <row r="43" spans="2:11">
+      <c r="B43" s="13"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="16"/>
+      <c r="H43" s="17"/>
+      <c r="I43" s="17"/>
+      <c r="J43" s="17"/>
+      <c r="K43" s="18"/>
+    </row>
+    <row r="44" spans="2:11">
+      <c r="B44" s="13"/>
+      <c r="C44" s="14"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="16"/>
+      <c r="H44" s="17"/>
+      <c r="I44" s="17"/>
+      <c r="J44" s="17"/>
+      <c r="K44" s="18"/>
+    </row>
+    <row r="45" spans="2:11">
+      <c r="B45" s="13"/>
+      <c r="C45" s="14"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="16"/>
+      <c r="H45" s="17"/>
+      <c r="I45" s="17"/>
+      <c r="J45" s="17"/>
+      <c r="K45" s="18"/>
+    </row>
+    <row r="46" spans="2:11">
+      <c r="B46" s="13"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="17"/>
+      <c r="I46" s="17"/>
+      <c r="J46" s="17"/>
+      <c r="K46" s="18"/>
+    </row>
+    <row r="47" spans="2:11">
+      <c r="B47" s="13"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="15"/>
+      <c r="G47" s="16"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="17"/>
+      <c r="J47" s="17"/>
+      <c r="K47" s="18"/>
+    </row>
+    <row r="48" spans="2:11">
+      <c r="B48" s="13"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="15"/>
+      <c r="G48" s="16"/>
+      <c r="H48" s="17"/>
+      <c r="I48" s="17"/>
+      <c r="J48" s="17"/>
+      <c r="K48" s="18"/>
+    </row>
+    <row r="49" spans="2:11" ht="15.75" thickBot="1">
+      <c r="B49" s="19"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="21"/>
+      <c r="G49" s="22"/>
+      <c r="H49" s="23"/>
+      <c r="I49" s="23"/>
+      <c r="J49" s="23"/>
+      <c r="K49" s="24"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="J3:J4"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B5:K49">
+    <cfRule type="expression" dxfId="14" priority="1">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5:C100 E5:E100">
+    <cfRule type="containsText" dxfId="13" priority="2" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",C5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="3" operator="containsText" text="—">
+      <formula>NOT(ISERROR(SEARCH("—",C5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="↓">
+      <formula>NOT(ISERROR(SEARCH("↓",C5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="5" operator="containsText" text="↑">
+      <formula>NOT(ISERROR(SEARCH("↑",C5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96A5A66E-8EC4-45E3-990B-C2EFEC6F74DB}">
+  <dimension ref="B1:J59"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="0.625" customWidth="1"/>
+    <col min="2" max="2" width="7.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="7.625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="21.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" style="2"/>
+    <col min="9" max="9" width="9" style="2" customWidth="1"/>
+    <col min="10" max="10" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" ht="4.5" customHeight="1" thickBot="1"/>
+    <row r="2" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B2" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="33"/>
+    </row>
+    <row r="3" spans="2:10">
+      <c r="B3" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="35"/>
+      <c r="D3" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="37"/>
+      <c r="F3" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="J3" s="44" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="39"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="45"/>
+    </row>
+    <row r="5" spans="2:10" ht="14.25" customHeight="1">
+      <c r="B5" s="25">
+        <v>1</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" s="25">
+        <v>1</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="29">
+        <v>9</v>
+      </c>
+      <c r="I5" s="29">
+        <v>3</v>
+      </c>
+      <c r="J5" s="30">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" ht="14.25" customHeight="1">
+      <c r="B6" s="13">
+        <v>1</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="D6" s="13">
+        <v>1</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="17">
+        <v>6</v>
+      </c>
+      <c r="I6" s="17">
+        <v>6</v>
+      </c>
+      <c r="J6" s="18">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" ht="15" customHeight="1">
+      <c r="B7" s="13">
+        <v>2</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="D7" s="13">
+        <v>3</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="17">
+        <v>6</v>
+      </c>
+      <c r="I7" s="17">
+        <v>3</v>
+      </c>
+      <c r="J7" s="18">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10">
+      <c r="B8" s="13">
+        <v>2</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D8" s="13">
+        <v>3</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="17">
+        <v>9</v>
+      </c>
+      <c r="I8" s="17">
+        <v>0</v>
+      </c>
+      <c r="J8" s="18">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10">
+      <c r="B9" s="13">
+        <v>2</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D9" s="13">
+        <v>3</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="17">
+        <v>9</v>
+      </c>
+      <c r="I9" s="17">
+        <v>0</v>
+      </c>
+      <c r="J9" s="18">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10">
+      <c r="B10" s="13">
+        <v>2</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" s="13">
+        <v>3</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="17">
+        <v>9</v>
+      </c>
+      <c r="I10" s="17">
+        <v>0</v>
+      </c>
+      <c r="J10" s="18">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10">
+      <c r="B11" s="13">
+        <v>2</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D11" s="13">
+        <v>3</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="17">
+        <v>9</v>
+      </c>
+      <c r="I11" s="17">
+        <v>0</v>
+      </c>
+      <c r="J11" s="18">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10">
+      <c r="B12" s="13">
+        <v>2</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="D12" s="13">
+        <v>3</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="17">
+        <v>6</v>
+      </c>
+      <c r="I12" s="17">
+        <v>3</v>
+      </c>
+      <c r="J12" s="18">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10">
+      <c r="B13" s="13">
+        <v>2</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="D13" s="13">
+        <v>3</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="17">
+        <v>6</v>
+      </c>
+      <c r="I13" s="17">
+        <v>3</v>
+      </c>
+      <c r="J13" s="18">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10">
+      <c r="B14" s="13">
+        <v>3</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="D14" s="13">
+        <v>10</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="H14" s="17">
+        <v>0</v>
+      </c>
+      <c r="I14" s="17">
+        <v>6</v>
+      </c>
+      <c r="J14" s="18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" ht="14.25" customHeight="1">
+      <c r="B15" s="13">
+        <v>3</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="D15" s="13">
+        <v>10</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="H15" s="17">
+        <v>3</v>
+      </c>
+      <c r="I15" s="17">
+        <v>3</v>
+      </c>
+      <c r="J15" s="18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" ht="14.25" customHeight="1">
+      <c r="B16" s="13">
+        <v>3</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="D16" s="13">
+        <v>10</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="H16" s="17">
+        <v>3</v>
+      </c>
+      <c r="I16" s="17">
+        <v>3</v>
+      </c>
+      <c r="J16" s="18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" ht="14.25" customHeight="1">
+      <c r="B17" s="13">
+        <v>3</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="D17" s="13">
+        <v>10</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="H17" s="17">
+        <v>3</v>
+      </c>
+      <c r="I17" s="17">
+        <v>3</v>
+      </c>
+      <c r="J17" s="18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="14.25" customHeight="1">
+      <c r="B18" s="13">
+        <v>3</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="D18" s="13">
+        <v>10</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="H18" s="17">
+        <v>3</v>
+      </c>
+      <c r="I18" s="17">
+        <v>3</v>
+      </c>
+      <c r="J18" s="18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10">
+      <c r="B19" s="13">
+        <v>3</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D19" s="13">
+        <v>10</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19" s="17">
+        <v>6</v>
+      </c>
+      <c r="I19" s="17">
+        <v>0</v>
+      </c>
+      <c r="J19" s="18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10">
+      <c r="B20" s="13">
+        <v>3</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="D20" s="13">
+        <v>10</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="G20" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="H20" s="17">
+        <v>3</v>
+      </c>
+      <c r="I20" s="17">
+        <v>3</v>
+      </c>
+      <c r="J20" s="18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10">
+      <c r="B21" s="13">
+        <v>3</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D21" s="13">
+        <v>10</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="H21" s="17">
+        <v>6</v>
+      </c>
+      <c r="I21" s="17">
+        <v>0</v>
+      </c>
+      <c r="J21" s="18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10">
+      <c r="B22" s="13">
+        <v>3</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="D22" s="13">
+        <v>10</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="G22" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="H22" s="17">
+        <v>3</v>
+      </c>
+      <c r="I22" s="17">
+        <v>3</v>
+      </c>
+      <c r="J22" s="18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10">
+      <c r="B23" s="13">
+        <v>3</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D23" s="13">
+        <v>10</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="G23" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="H23" s="17">
+        <v>6</v>
+      </c>
+      <c r="I23" s="17">
+        <v>0</v>
+      </c>
+      <c r="J23" s="18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10">
+      <c r="B24" s="13">
+        <v>4</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="D24" s="13">
+        <v>20</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="H24" s="17">
+        <v>0</v>
+      </c>
+      <c r="I24" s="17">
+        <v>3</v>
+      </c>
+      <c r="J24" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10">
+      <c r="B25" s="13">
+        <v>4</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="D25" s="13">
+        <v>20</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G25" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="H25" s="17">
+        <v>0</v>
+      </c>
+      <c r="I25" s="17">
+        <v>3</v>
+      </c>
+      <c r="J25" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10">
+      <c r="B26" s="13">
+        <v>4</v>
+      </c>
+      <c r="C26" s="46" t="s">
+        <v>101</v>
+      </c>
+      <c r="D26" s="13">
+        <v>20</v>
+      </c>
+      <c r="E26" s="46" t="s">
+        <v>108</v>
+      </c>
+      <c r="F26" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="G26" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="H26" s="49">
+        <v>3</v>
+      </c>
+      <c r="I26" s="49">
+        <v>0</v>
+      </c>
+      <c r="J26" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10">
+      <c r="B27" s="13">
+        <v>4</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D27" s="13">
+        <v>20</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G27" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="H27" s="17">
+        <v>3</v>
+      </c>
+      <c r="I27" s="17">
+        <v>0</v>
+      </c>
+      <c r="J27" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10">
+      <c r="B28" s="13">
+        <v>4</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D28" s="13">
+        <v>20</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="G28" s="16"/>
+      <c r="H28" s="17">
+        <v>3</v>
+      </c>
+      <c r="I28" s="17">
+        <v>0</v>
+      </c>
+      <c r="J28" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10">
+      <c r="B29" s="13">
+        <v>4</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D29" s="13">
+        <v>20</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="G29" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="H29" s="17">
+        <v>3</v>
+      </c>
+      <c r="I29" s="17">
+        <v>0</v>
+      </c>
+      <c r="J29" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10">
+      <c r="B30" s="13">
+        <v>4</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D30" s="13">
+        <v>20</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="F30" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="G30" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="H30" s="17">
+        <v>3</v>
+      </c>
+      <c r="I30" s="17">
+        <v>0</v>
+      </c>
+      <c r="J30" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10">
+      <c r="B31" s="13">
+        <v>4</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="13">
+        <v>20</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="G31" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="H31" s="17">
+        <v>0</v>
+      </c>
+      <c r="I31" s="17">
+        <v>3</v>
+      </c>
+      <c r="J31" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10">
+      <c r="B32" s="13">
+        <v>4</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="D32" s="13">
+        <v>20</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="G32" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="H32" s="17">
+        <v>0</v>
+      </c>
+      <c r="I32" s="17">
+        <v>3</v>
+      </c>
+      <c r="J32" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10">
+      <c r="B33" s="13">
+        <v>4</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D33" s="13">
+        <v>20</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="F33" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="G33" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="H33" s="17">
+        <v>3</v>
+      </c>
+      <c r="I33" s="17">
+        <v>0</v>
+      </c>
+      <c r="J33" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10">
+      <c r="B34" s="13">
+        <v>4</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D34" s="13">
+        <v>20</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="F34" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="G34" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="H34" s="17">
+        <v>3</v>
+      </c>
+      <c r="I34" s="17">
+        <v>0</v>
+      </c>
+      <c r="J34" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10">
+      <c r="B35" s="13">
+        <v>4</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D35" s="13">
+        <v>20</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="F35" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="G35" s="16"/>
+      <c r="H35" s="17">
+        <v>3</v>
+      </c>
+      <c r="I35" s="17">
+        <v>0</v>
+      </c>
+      <c r="J35" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10">
+      <c r="B36" s="13">
+        <v>5</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" s="13">
+        <v>32</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="G36" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="H36" s="17">
+        <v>0</v>
+      </c>
+      <c r="I36" s="17">
+        <v>0</v>
+      </c>
+      <c r="J36" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10">
+      <c r="B37" s="13">
+        <v>5</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D37" s="13">
+        <v>32</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="F37" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="G37" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="H37" s="17">
+        <v>0</v>
+      </c>
+      <c r="I37" s="17">
+        <v>0</v>
+      </c>
+      <c r="J37" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10">
+      <c r="B38" s="13">
+        <v>5</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" s="13">
+        <v>32</v>
+      </c>
+      <c r="E38" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="G38" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="H38" s="17">
+        <v>0</v>
+      </c>
+      <c r="I38" s="17">
+        <v>0</v>
+      </c>
+      <c r="J38" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10">
+      <c r="B39" s="13">
+        <v>5</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D39" s="13">
+        <v>32</v>
+      </c>
+      <c r="E39" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="F39" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G39" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="H39" s="17">
+        <v>0</v>
+      </c>
+      <c r="I39" s="17">
+        <v>0</v>
+      </c>
+      <c r="J39" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10">
+      <c r="B40" s="13">
+        <v>5</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D40" s="13">
+        <v>32</v>
+      </c>
+      <c r="E40" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="F40" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="G40" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="H40" s="17">
+        <v>0</v>
+      </c>
+      <c r="I40" s="17">
+        <v>0</v>
+      </c>
+      <c r="J40" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10">
+      <c r="B41" s="13">
+        <v>5</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="13">
+        <v>32</v>
+      </c>
+      <c r="E41" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="G41" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="H41" s="17">
+        <v>0</v>
+      </c>
+      <c r="I41" s="17">
+        <v>0</v>
+      </c>
+      <c r="J41" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10">
+      <c r="B42" s="13">
+        <v>5</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D42" s="13">
+        <v>32</v>
+      </c>
+      <c r="E42" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="F42" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="G42" s="16"/>
+      <c r="H42" s="17">
+        <v>0</v>
+      </c>
+      <c r="I42" s="17">
+        <v>0</v>
+      </c>
+      <c r="J42" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10">
+      <c r="B43" s="13">
+        <v>5</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43" s="13">
+        <v>32</v>
+      </c>
+      <c r="E43" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="G43" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="H43" s="17">
+        <v>0</v>
+      </c>
+      <c r="I43" s="17">
+        <v>0</v>
+      </c>
+      <c r="J43" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10">
+      <c r="B44" s="13">
+        <v>5</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D44" s="13">
+        <v>32</v>
+      </c>
+      <c r="E44" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F44" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="G44" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="H44" s="17">
+        <v>0</v>
+      </c>
+      <c r="I44" s="17">
+        <v>0</v>
+      </c>
+      <c r="J44" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10">
+      <c r="B45" s="13">
+        <v>5</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D45" s="13">
+        <v>32</v>
+      </c>
+      <c r="E45" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="F45" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="G45" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="H45" s="17">
+        <v>0</v>
+      </c>
+      <c r="I45" s="17">
+        <v>0</v>
+      </c>
+      <c r="J45" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10">
+      <c r="B46" s="13">
+        <v>5</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D46" s="13">
+        <v>32</v>
+      </c>
+      <c r="E46" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="F46" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="G46" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="H46" s="17">
+        <v>0</v>
+      </c>
+      <c r="I46" s="17">
+        <v>0</v>
+      </c>
+      <c r="J46" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10">
+      <c r="B47" s="13">
+        <v>5</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D47" s="13">
+        <v>32</v>
+      </c>
+      <c r="E47" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F47" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="G47" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="H47" s="17">
+        <v>0</v>
+      </c>
+      <c r="I47" s="17">
+        <v>0</v>
+      </c>
+      <c r="J47" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10">
+      <c r="B48" s="13">
+        <v>5</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D48" s="13">
+        <v>32</v>
+      </c>
+      <c r="E48" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F48" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="G48" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="H48" s="17">
+        <v>0</v>
+      </c>
+      <c r="I48" s="17">
+        <v>0</v>
+      </c>
+      <c r="J48" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="2:10">
+      <c r="B49" s="13">
+        <v>5</v>
+      </c>
+      <c r="C49" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D49" s="13">
+        <v>32</v>
+      </c>
+      <c r="E49" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="F49" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="G49" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="H49" s="17">
+        <v>0</v>
+      </c>
+      <c r="I49" s="17">
+        <v>0</v>
+      </c>
+      <c r="J49" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10">
+      <c r="B50" s="13">
+        <v>5</v>
+      </c>
+      <c r="C50" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D50" s="13">
+        <v>32</v>
+      </c>
+      <c r="E50" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="F50" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="G50" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="H50" s="17">
+        <v>0</v>
+      </c>
+      <c r="I50" s="17">
+        <v>0</v>
+      </c>
+      <c r="J50" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10">
+      <c r="B51" s="13">
+        <v>5</v>
+      </c>
+      <c r="C51" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D51" s="13">
+        <v>32</v>
+      </c>
+      <c r="E51" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="F51" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="G51" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="H51" s="17">
+        <v>0</v>
+      </c>
+      <c r="I51" s="17">
+        <v>0</v>
+      </c>
+      <c r="J51" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10">
+      <c r="B52" s="13">
+        <v>5</v>
+      </c>
+      <c r="C52" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D52" s="13">
+        <v>32</v>
+      </c>
+      <c r="E52" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F52" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="G52" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="H52" s="17">
+        <v>0</v>
+      </c>
+      <c r="I52" s="17">
+        <v>0</v>
+      </c>
+      <c r="J52" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="2:10">
+      <c r="B53" s="13">
+        <v>5</v>
+      </c>
+      <c r="C53" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D53" s="13">
+        <v>32</v>
+      </c>
+      <c r="E53" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="F53" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="G53" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="H53" s="17">
+        <v>0</v>
+      </c>
+      <c r="I53" s="17">
+        <v>0</v>
+      </c>
+      <c r="J53" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="2:10">
+      <c r="B54" s="13">
+        <v>5</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D54" s="13">
+        <v>32</v>
+      </c>
+      <c r="E54" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="F54" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="G54" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="H54" s="17">
+        <v>0</v>
+      </c>
+      <c r="I54" s="17">
+        <v>0</v>
+      </c>
+      <c r="J54" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="2:10">
+      <c r="B55" s="13">
+        <v>5</v>
+      </c>
+      <c r="C55" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D55" s="13">
+        <v>32</v>
+      </c>
+      <c r="E55" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="F55" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="G55" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="H55" s="17">
+        <v>0</v>
+      </c>
+      <c r="I55" s="17">
+        <v>0</v>
+      </c>
+      <c r="J55" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="2:10">
+      <c r="B56" s="13">
+        <v>5</v>
+      </c>
+      <c r="C56" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D56" s="13">
+        <v>32</v>
+      </c>
+      <c r="E56" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="F56" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="G56" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="H56" s="17">
+        <v>0</v>
+      </c>
+      <c r="I56" s="17">
+        <v>0</v>
+      </c>
+      <c r="J56" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="2:10">
+      <c r="B57" s="13">
+        <v>5</v>
+      </c>
+      <c r="C57" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D57" s="13">
+        <v>32</v>
+      </c>
+      <c r="E57" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="F57" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="G57" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="H57" s="17">
+        <v>0</v>
+      </c>
+      <c r="I57" s="17">
+        <v>0</v>
+      </c>
+      <c r="J57" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="2:10">
+      <c r="B58" s="13">
+        <v>5</v>
+      </c>
+      <c r="C58" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D58" s="13">
+        <v>32</v>
+      </c>
+      <c r="E58" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F58" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="G58" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="H58" s="17">
+        <v>0</v>
+      </c>
+      <c r="I58" s="17">
+        <v>0</v>
+      </c>
+      <c r="J58" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B59" s="19">
+        <v>5</v>
+      </c>
+      <c r="C59" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="D59" s="19">
+        <v>32</v>
+      </c>
+      <c r="E59" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="F59" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="G59" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="H59" s="23">
+        <v>0</v>
+      </c>
+      <c r="I59" s="23">
+        <v>0</v>
+      </c>
+      <c r="J59" s="24">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="I3:I4"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B5:J59">
+    <cfRule type="expression" dxfId="9" priority="1">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5:C110 E5:E110">
+    <cfRule type="containsText" dxfId="8" priority="2" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",C5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="—">
+      <formula>NOT(ISERROR(SEARCH("—",C5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="↓">
+      <formula>NOT(ISERROR(SEARCH("↓",C5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="↑">
+      <formula>NOT(ISERROR(SEARCH("↑",C5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEBB9A6D-0090-4854-BAF2-388FE86374DA}">
   <dimension ref="B1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
@@ -1192,36 +3772,36 @@
   <sheetData>
     <row r="1" spans="2:9" ht="4.5" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="27"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="33"/>
     </row>
     <row r="3" spans="2:9">
-      <c r="B3" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="30" t="s">
+      <c r="B3" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="35"/>
+      <c r="D3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="31"/>
-      <c r="F3" s="32" t="s">
+      <c r="E3" s="37"/>
+      <c r="F3" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="34" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3" s="38" t="s">
+      <c r="G3" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="36" t="s">
+      <c r="I3" s="44" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1238,10 +3818,10 @@
       <c r="E4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="33"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="37"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="45"/>
     </row>
     <row r="5" spans="2:9" ht="14.25" customHeight="1">
       <c r="B5" s="7">

</xml_diff>